<commit_message>
notitie toegevoegd dat gemeentecode 2 nep is & weg moet wanneer echte data beschikbaar is.
</commit_message>
<xml_diff>
--- a/JongVolwassenenNaarGeslachtEnLeeftijd1Jan2024.xlsx
+++ b/JongVolwassenenNaarGeslachtEnLeeftijd1Jan2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetservicecentrum.sharepoint.com/sites/hvbtonderzoek/Shared Documents/Data gedreven/gmjv-landelijk-format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_606378D0329A772147AB5256E6820B9E95DC8B12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93D7E7FF-DAAB-4873-9D55-0F59031D85E2}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_606378D0329A772147AB5256E6820B9E95DC8B12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21714300-4224-47F2-8A81-E48353E09336}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="795">
   <si>
     <t>Man</t>
   </si>
@@ -2411,6 +2411,9 @@
   </si>
   <si>
     <t>NepgemeenteB</t>
+  </si>
+  <si>
+    <t>LET OP groningen tijdelijk als "nepgemeenteB" neergezet t.b.v. testen</t>
   </si>
 </sst>
 </file>
@@ -4534,10 +4537,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I348"/>
+  <dimension ref="A1:K348"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4548,7 +4551,7 @@
     <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>726</v>
       </c>
@@ -4557,7 +4560,7 @@
       <c r="D1" s="25"/>
       <c r="E1" s="25"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>780</v>
       </c>
@@ -4572,7 +4575,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C5" s="20" t="s">
         <v>0</v>
       </c>
@@ -4581,7 +4584,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>711</v>
       </c>
@@ -4590,7 +4593,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C7" s="20" t="s">
         <v>720</v>
       </c>
@@ -4611,7 +4614,7 @@
       </c>
       <c r="I7" s="20"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>782</v>
       </c>
@@ -4640,7 +4643,7 @@
         <v>1435</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -4668,8 +4671,11 @@
       <c r="I9">
         <v>58979</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -4698,7 +4704,7 @@
         <v>27607</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -4727,7 +4733,7 @@
         <v>3471</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -4756,7 +4762,7 @@
         <v>3047</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -4785,7 +4791,7 @@
         <v>3035</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -4814,7 +4820,7 @@
         <v>3463</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -4843,7 +4849,7 @@
         <v>1733</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -14486,6 +14492,65 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Standaard document" ma:contentTypeID="0x01010032BFCF0B4ED1F248A04F0BC4CDA2D40E004922E14A0C99784589A2C683F8449396" ma:contentTypeVersion="23" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="0fc91688edb3432943f87096013952fa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2a4b34cd-775e-401e-bc6c-0ba6e02713bb" xmlns:ns3="5cd3556a-8845-4381-9ab1-80dc7cf34289" xmlns:ns4="3f7c12ff-62a7-41e2-b7c4-57e3c85fe2ec" xmlns:ns5="8079d392-526f-40d2-b8ec-fbb67b4a63f0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="74c553c88de14bc0c8b85e53e9537796" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="2a4b34cd-775e-401e-bc6c-0ba6e02713bb"/>
@@ -14886,65 +14951,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -14966,17 +14972,33 @@
         <AccountType/>
       </UserInfo>
     </GgdPractitioner>
-    <_dlc_DocId xmlns="2a4b34cd-775e-401e-bc6c-0ba6e02713bb">HVBDOC-2105918694-132891</_dlc_DocId>
+    <_dlc_DocId xmlns="2a4b34cd-775e-401e-bc6c-0ba6e02713bb">HVBDOC-2105918694-136990</_dlc_DocId>
     <_dlc_DocIdUrl xmlns="2a4b34cd-775e-401e-bc6c-0ba6e02713bb">
-      <Url>https://hetservicecentrum.sharepoint.com/sites/hvbtonderzoek/_layouts/15/DocIdRedir.aspx?ID=HVBDOC-2105918694-132891</Url>
-      <Description>HVBDOC-2105918694-132891</Description>
+      <Url>https://hetservicecentrum.sharepoint.com/sites/hvbtonderzoek/_layouts/15/DocIdRedir.aspx?ID=HVBDOC-2105918694-136990</Url>
+      <Description>HVBDOC-2105918694-136990</Description>
     </_dlc_DocIdUrl>
   </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53B8E88F-3A16-4B52-B489-450E18B59777}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3E716A0-A53C-4883-9BCC-C190FA45A77D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4594C01-CCBE-4789-A324-9D0CCA4AE597}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC5D478C-E667-46E7-AAC7-942EF8F478D8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -14996,22 +15018,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4594C01-CCBE-4789-A324-9D0CCA4AE597}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3E716A0-A53C-4883-9BCC-C190FA45A77D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD8B2D73-A82B-45D8-A4B7-8A3145E61C9C}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
responstabel toelichting kleuren uitgebreid
</commit_message>
<xml_diff>
--- a/JongVolwassenenNaarGeslachtEnLeeftijd1Jan2024.xlsx
+++ b/JongVolwassenenNaarGeslachtEnLeeftijd1Jan2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetservicecentrum.sharepoint.com/sites/hvbtonderzoek/Shared Documents/Data gedreven/gmjv-landelijk-format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_606378D0329A772147AB5256E6820B9E95DC8B12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21714300-4224-47F2-8A81-E48353E09336}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_606378D0329A772147AB5256E6820B9E95DC8B12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DAA114F-0AB5-411B-B0F8-BE9F6E118599}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="795">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="794">
   <si>
     <t>Man</t>
   </si>
@@ -2411,9 +2411,6 @@
   </si>
   <si>
     <t>NepgemeenteB</t>
-  </si>
-  <si>
-    <t>LET OP groningen tijdelijk als "nepgemeenteB" neergezet t.b.v. testen</t>
   </si>
 </sst>
 </file>
@@ -4537,10 +4534,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:K348"/>
+  <dimension ref="A1:I348"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4551,7 +4548,7 @@
     <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>726</v>
       </c>
@@ -4560,7 +4557,7 @@
       <c r="D1" s="25"/>
       <c r="E1" s="25"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>780</v>
       </c>
@@ -4575,7 +4572,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C5" s="20" t="s">
         <v>0</v>
       </c>
@@ -4584,7 +4581,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>711</v>
       </c>
@@ -4593,7 +4590,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C7" s="20" t="s">
         <v>720</v>
       </c>
@@ -4614,7 +4611,7 @@
       </c>
       <c r="I7" s="20"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>782</v>
       </c>
@@ -4643,7 +4640,7 @@
         <v>1435</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -4671,11 +4668,8 @@
       <c r="I9">
         <v>58979</v>
       </c>
-      <c r="K9" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -4704,7 +4698,7 @@
         <v>27607</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -4733,7 +4727,7 @@
         <v>3471</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -4762,7 +4756,7 @@
         <v>3047</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -4791,7 +4785,7 @@
         <v>3035</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -4820,7 +4814,7 @@
         <v>3463</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -4849,7 +4843,7 @@
         <v>1733</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -14492,65 +14486,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Standaard document" ma:contentTypeID="0x01010032BFCF0B4ED1F248A04F0BC4CDA2D40E004922E14A0C99784589A2C683F8449396" ma:contentTypeVersion="23" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="0fc91688edb3432943f87096013952fa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2a4b34cd-775e-401e-bc6c-0ba6e02713bb" xmlns:ns3="5cd3556a-8845-4381-9ab1-80dc7cf34289" xmlns:ns4="3f7c12ff-62a7-41e2-b7c4-57e3c85fe2ec" xmlns:ns5="8079d392-526f-40d2-b8ec-fbb67b4a63f0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="74c553c88de14bc0c8b85e53e9537796" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="2a4b34cd-775e-401e-bc6c-0ba6e02713bb"/>
@@ -14951,6 +14886,65 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -14982,22 +14976,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3E716A0-A53C-4883-9BCC-C190FA45A77D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4594C01-CCBE-4789-A324-9D0CCA4AE597}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC5D478C-E667-46E7-AAC7-942EF8F478D8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15018,6 +14996,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4594C01-CCBE-4789-A324-9D0CCA4AE597}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3E716A0-A53C-4883-9BCC-C190FA45A77D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD8B2D73-A82B-45D8-A4B7-8A3145E61C9C}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Lettertype ggplot aangepast naar "Open Sans". Hiervoor andere graphic device aangeroepen via library 'showtext'.
</commit_message>
<xml_diff>
--- a/JongVolwassenenNaarGeslachtEnLeeftijd1Jan2024.xlsx
+++ b/JongVolwassenenNaarGeslachtEnLeeftijd1Jan2024.xlsx
@@ -14700,4 +14700,510 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Standaard document" ma:contentTypeID="0x01010032BFCF0B4ED1F248A04F0BC4CDA2D40E004922E14A0C99784589A2C683F8449396" ma:contentTypeVersion="23" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="0fc91688edb3432943f87096013952fa">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2a4b34cd-775e-401e-bc6c-0ba6e02713bb" xmlns:ns3="5cd3556a-8845-4381-9ab1-80dc7cf34289" xmlns:ns4="3f7c12ff-62a7-41e2-b7c4-57e3c85fe2ec" xmlns:ns5="8079d392-526f-40d2-b8ec-fbb67b4a63f0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="74c553c88de14bc0c8b85e53e9537796" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
+    <xsd:import namespace="2a4b34cd-775e-401e-bc6c-0ba6e02713bb"/>
+    <xsd:import namespace="5cd3556a-8845-4381-9ab1-80dc7cf34289"/>
+    <xsd:import namespace="3f7c12ff-62a7-41e2-b7c4-57e3c85fe2ec"/>
+    <xsd:import namespace="8079d392-526f-40d2-b8ec-fbb67b4a63f0"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:Proces" minOccurs="0"/>
+                <xsd:element ref="ns2:Documentstatus" minOccurs="0"/>
+                <xsd:element ref="ns3:GgdPractitioner" minOccurs="0"/>
+                <xsd:element ref="ns4:GgdStartDate" minOccurs="0"/>
+                <xsd:element ref="ns4:GgdEndDate" minOccurs="0"/>
+                <xsd:element ref="ns4:GgdPractitionerStatus" minOccurs="0"/>
+                <xsd:element ref="ns2:Organisatie" minOccurs="0"/>
+                <xsd:element ref="ns2:Gecontroleerd_x0020_door_x0020_informatiebeheer" minOccurs="0"/>
+                <xsd:element ref="ns2:_dlc_DocIdUrl" minOccurs="0"/>
+                <xsd:element ref="ns2:_dlc_DocIdPersistId" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns2:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:_dlc_DocId" minOccurs="0"/>
+                <xsd:element ref="ns5:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAllLabel" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2a4b34cd-775e-401e-bc6c-0ba6e02713bb" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="Proces" ma:index="2" nillable="true" ma:displayName="Proces" ma:internalName="Proces">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Adressenbeheer (1 jaar)"/>
+          <xsd:enumeration value="Advisering bij interne en externe organisaties, instellingen en evenementen (5 jaar)"/>
+          <xsd:enumeration value="Afhandeling van publieksvragen (1 jaar)"/>
+          <xsd:enumeration value="Bestuur en beleid (Permanent bewaren)"/>
+          <xsd:enumeration value="Contractbeheer (10 jaar)"/>
+          <xsd:enumeration value="Corrigerende en preventieve maatregelen (Permanent bewaren)"/>
+          <xsd:enumeration value="Extern overleg voeren (secretariaat bij andere organisatie) (1 jaar)"/>
+          <xsd:enumeration value="Extern overleg voeren (secretariaat voerend) (Permanent bewaren)"/>
+          <xsd:enumeration value="Externe audits (Permanent bewaren)"/>
+          <xsd:enumeration value="Externe communicatie (Permanent bewaren)"/>
+          <xsd:enumeration value="Externe klachtbehandeling (5 jaar)"/>
+          <xsd:enumeration value="Externe klachtbehandeling (5 jaar)"/>
+          <xsd:enumeration value="Externe klachtbehandeling na advies externe klachtencommissie (10 jaar)"/>
+          <xsd:enumeration value="Gezondheidsonderzoek uitvoeren (Permanent bewaren)"/>
+          <xsd:enumeration value="Hotspot (Permanent bewaren)"/>
+          <xsd:enumeration value="Huisstijl beheren (Permanent bewaren)"/>
+          <xsd:enumeration value="Interne (team)overleggen (1 jaar)"/>
+          <xsd:enumeration value="Interne audits (10 jaar)"/>
+          <xsd:enumeration value="Klant(tevredenheids)onderzoek (10 jaar)"/>
+          <xsd:enumeration value="Managementrapportages (7 jaar)"/>
+          <xsd:enumeration value="Opleiden en trainen van externen (5 jaar)"/>
+          <xsd:enumeration value="Opleiden, trainen, voorlichten en oefenen van eigen medewerkers (5 jaar)"/>
+          <xsd:enumeration value="Organiseren van activiteiten voor personeel (7 jaar)"/>
+          <xsd:enumeration value="Planning en roosters opstellen (7 jaar)"/>
+          <xsd:enumeration value="Planning, control en rapportage (Permanent bewaren)"/>
+          <xsd:enumeration value="Procesbeschrijvingen (Permanent bewaren)"/>
+          <xsd:enumeration value="Projecten uitvoeren (Afhankelijk van onderwerp)"/>
+          <xsd:enumeration value="Protocollen (10 jaar)"/>
+          <xsd:enumeration value="Risicomanagement (10 jaar)"/>
+          <xsd:enumeration value="Stageplaatsen organiseren (10 jaar)"/>
+          <xsd:enumeration value="Verkoopcontracten en Subsidieaanvragen (10 jaar)"/>
+          <xsd:enumeration value="Werkinstructies (5 jaar)"/>
+          <xsd:enumeration value="Werving van personeel (10 jaar)"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Documentstatus" ma:index="3" nillable="true" ma:displayName="Documentstatus" ma:internalName="Documentstatus">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Concept"/>
+          <xsd:enumeration value="Definitief"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Organisatie" ma:index="8" nillable="true" ma:displayName="Organisatie" ma:default="HVB" ma:internalName="Organisatie">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="HSC"/>
+          <xsd:enumeration value="HVB"/>
+          <xsd:enumeration value="NOG"/>
+          <xsd:enumeration value="RAV"/>
+          <xsd:enumeration value="WB"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Gecontroleerd_x0020_door_x0020_informatiebeheer" ma:index="9" nillable="true" ma:displayName="Gecontroleerd door informatiebeheer" ma:internalName="Gecontroleerd_x0020_door_x0020_informatiebeheer">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Ja"/>
+          <xsd:enumeration value="Nee"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_dlc_DocIdUrl" ma:index="11" nillable="true" ma:displayName="Document-id" ma:description="Permanent link to this document." ma:hidden="true" ma:internalName="_dlc_DocIdUrl" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:URL">
+            <xsd:sequence>
+              <xsd:element name="Url" type="dms:ValidUrl" minOccurs="0" nillable="true"/>
+              <xsd:element name="Description" type="xsd:string" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="_dlc_DocIdPersistId" ma:index="12" nillable="true" ma:displayName="Persist ID" ma:description="Keep ID on add." ma:hidden="true" ma:internalName="_dlc_DocIdPersistId" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharedWithUsers" ma:index="24" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="25" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_dlc_DocId" ma:index="26" nillable="true" ma:displayName="Waarde van de document-id" ma:description="The value of the document ID assigned to this item." ma:internalName="_dlc_DocId" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="32" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{4a7618aa-82f0-4f19-88dd-5125bb5b5123}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="2a4b34cd-775e-401e-bc6c-0ba6e02713bb">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAllLabel" ma:index="33" nillable="true" ma:displayName="Taxonomy Catch All Column1" ma:hidden="true" ma:list="{4a7618aa-82f0-4f19-88dd-5125bb5b5123}" ma:internalName="TaxCatchAllLabel" ma:readOnly="true" ma:showField="CatchAllDataLabel" ma:web="2a4b34cd-775e-401e-bc6c-0ba6e02713bb">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="5cd3556a-8845-4381-9ab1-80dc7cf34289" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="GgdPractitioner" ma:index="4" nillable="true" ma:displayName="Behandelaar" ma:list="UserInfo" ma:SharePointGroup="0" ma:internalName="GgdPractitioner" ma:showField="ImnName">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:User">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="3f7c12ff-62a7-41e2-b7c4-57e3c85fe2ec" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="GgdStartDate" ma:index="5" nillable="true" ma:displayName="Startdatum" ma:format="DateOnly" ma:internalName="GgdStartDate">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="GgdEndDate" ma:index="6" nillable="true" ma:displayName="Afhandeldatum" ma:format="DateOnly" ma:internalName="GgdEndDate">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="GgdPractitionerStatus" ma:index="7" nillable="true" ma:displayName="Behandelstatus" ma:format="Dropdown" ma:internalName="GgdPractitionerStatus">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="In behandeling"/>
+          <xsd:enumeration value="Afgehandeld"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="8079d392-526f-40d2-b8ec-fbb67b4a63f0" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="13" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="14" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="15" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="16" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="17" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="18" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="19" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="20" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="21" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="22" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="23" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="27" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="8cd2f11b-e0e3-409a-841c-e0a0fdabfd77" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="30" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="2a4b34cd-775e-401e-bc6c-0ba6e02713bb">HVBDOC-2105918694-136990</_dlc_DocId>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8079d392-526f-40d2-b8ec-fbb67b4a63f0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2a4b34cd-775e-401e-bc6c-0ba6e02713bb" xsi:nil="true"/>
+    <_dlc_DocIdUrl xmlns="2a4b34cd-775e-401e-bc6c-0ba6e02713bb">
+      <Url>https://hetservicecentrum.sharepoint.com/sites/hvbtonderzoek/_layouts/15/DocIdRedir.aspx?ID=HVBDOC-2105918694-136990</Url>
+      <Description>HVBDOC-2105918694-136990</Description>
+    </_dlc_DocIdUrl>
+    <Proces xmlns="2a4b34cd-775e-401e-bc6c-0ba6e02713bb" xsi:nil="true"/>
+    <GgdPractitionerStatus xmlns="3f7c12ff-62a7-41e2-b7c4-57e3c85fe2ec" xsi:nil="true"/>
+    <GgdEndDate xmlns="3f7c12ff-62a7-41e2-b7c4-57e3c85fe2ec" xsi:nil="true"/>
+    <Organisatie xmlns="2a4b34cd-775e-401e-bc6c-0ba6e02713bb">HVB</Organisatie>
+    <Documentstatus xmlns="2a4b34cd-775e-401e-bc6c-0ba6e02713bb" xsi:nil="true"/>
+    <GgdStartDate xmlns="3f7c12ff-62a7-41e2-b7c4-57e3c85fe2ec" xsi:nil="true"/>
+    <Gecontroleerd_x0020_door_x0020_informatiebeheer xmlns="2a4b34cd-775e-401e-bc6c-0ba6e02713bb" xsi:nil="true"/>
+    <GgdPractitioner xmlns="5cd3556a-8845-4381-9ab1-80dc7cf34289">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </GgdPractitioner>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC6AE0F2-4277-427D-8E9B-15CE4EC7C1DE}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65056DA5-1A96-461D-A32D-1BD5A46BCD42}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F177D77B-3F72-4414-AB22-6039153C9143}"/>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EC95B05-C2A1-4052-94CB-515880A7DAB6}"/>
 </file>
</xml_diff>